<commit_message>
added inductor to part list, Mann!
</commit_message>
<xml_diff>
--- a/Hardware/MidiSwitchPCB/PartList.xlsx
+++ b/Hardware/MidiSwitchPCB/PartList.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="149">
   <si>
     <t>Partl</t>
   </si>
@@ -475,6 +475,15 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.mouser.de/ProductDetail/Broadcom-Avago/6N138-500E?qs=sGAEpiMZZMtd3yBnp8bAgMhsn5Iee23BCIxIH5VeXTY%3D </t>
+  </si>
+  <si>
+    <t>Vorhanden</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Taiyo-Yuden/NRS8030T4R7MJGJ?qs=sGAEpiMZZMsg%252By3WlYCkU5iuzh4MJmq0OBV6vXuK5mk%3D</t>
+  </si>
+  <si>
+    <t>963-NRS8030T4R7MJGJ</t>
   </si>
 </sst>
 </file>
@@ -831,7 +840,7 @@
   <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="B23" sqref="A23:XFD31"/>
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,6 +988,9 @@
       <c r="G13">
         <v>1</v>
       </c>
+      <c r="I13" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1019,6 +1031,9 @@
       <c r="G15">
         <v>1</v>
       </c>
+      <c r="I15" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1039,6 +1054,9 @@
       <c r="G16">
         <v>1</v>
       </c>
+      <c r="I16" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1528,6 +1546,12 @@
       </c>
       <c r="G42">
         <v>1</v>
+      </c>
+      <c r="H42" t="s">
+        <v>148</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2207,6 +2231,7 @@
     <hyperlink ref="I45" r:id="rId1"/>
     <hyperlink ref="I23" r:id="rId2"/>
     <hyperlink ref="I43" r:id="rId3"/>
+    <hyperlink ref="I42" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added switching capacitor to part list (changed cap-package in layout from 0603 to 1206)
</commit_message>
<xml_diff>
--- a/Hardware/MidiSwitchPCB/PartList.xlsx
+++ b/Hardware/MidiSwitchPCB/PartList.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="153">
   <si>
     <t>Partl</t>
   </si>
@@ -484,6 +484,18 @@
   </si>
   <si>
     <t>963-NRS8030T4R7MJGJ</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Murata-Electronics/GRM31C5C1E104JA01K?qs=%2Fha2pyFaduhBfEIR6jcOaJ56CU6eddb5oLEFH%252BIY%2FeBTD895l24yhA%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81-GRM31C5C1E104JA1K </t>
+  </si>
+  <si>
+    <t>C1206</t>
+  </si>
+  <si>
+    <t>C-EUC1206 Zwitschi-Cap</t>
   </si>
 </sst>
 </file>
@@ -839,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,10 +1032,10 @@
         <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>152</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>151</v>
       </c>
       <c r="F15" t="s">
         <v>24</v>
@@ -1031,8 +1043,11 @@
       <c r="G15">
         <v>1</v>
       </c>
+      <c r="H15" t="s">
+        <v>150</v>
+      </c>
       <c r="I15" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1043,10 +1058,10 @@
         <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>152</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>151</v>
       </c>
       <c r="F16" t="s">
         <v>24</v>
@@ -1054,8 +1069,11 @@
       <c r="G16">
         <v>1</v>
       </c>
+      <c r="H16" t="s">
+        <v>150</v>
+      </c>
       <c r="I16" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>